<commit_message>
going to flood the top!
</commit_message>
<xml_diff>
--- a/l2_dev_alternative _nopwrsense/BOM.xlsx
+++ b/l2_dev_alternative _nopwrsense/BOM.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="l2_dev_board-25-08-11" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -348,7 +348,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -843,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1183,7 +1183,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>